<commit_message>
Drop an entry for space
</commit_message>
<xml_diff>
--- a/cv_data/publications.xlsx
+++ b/cv_data/publications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cclan\OneDrive\GitHub\ccl_cv\cv_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="179" documentId="8_{4CB552C3-CF36-4963-A779-1A56A658881C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F11B9B54-63E8-4270-8A5C-40E88AEADC43}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{4CB552C3-CF36-4963-A779-1A56A658881C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B5451723-44DF-47B8-945C-8CED90FF4905}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{89DB09BC-2BA0-43D2-AE3C-68FBD892520E}"/>
+    <workbookView xWindow="41250" yWindow="765" windowWidth="28800" windowHeight="14775" xr2:uid="{89DB09BC-2BA0-43D2-AE3C-68FBD892520E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>type</t>
   </si>
@@ -256,9 +256,6 @@
   </si>
   <si>
     <t>The Effect of a Gas Shortage on Transit Use in Mexico City and Guadalajara</t>
-  </si>
-  <si>
-    <t>Family Dynamics, Birth Timing, and Child Temperament: A Dynamic Sibling Model Approach</t>
   </si>
 </sst>
 </file>
@@ -632,7 +629,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,18 +1037,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>77</v>
-      </c>
+      <c r="D21" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>